<commit_message>
anwendungsdaten für testlauf optimiert
</commit_message>
<xml_diff>
--- a/doc/anforderungenAbfragen.xlsx
+++ b/doc/anforderungenAbfragen.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="88">
   <si>
     <t>Anforderungen</t>
   </si>
@@ -193,6 +193,93 @@
   </si>
   <si>
     <t>flächenmäßige Veränderung Penzlin (13056053) von 2000 bis 2011</t>
+  </si>
+  <si>
+    <t>alle Umzüge aus Oberzentren MV in ABL</t>
+  </si>
+  <si>
+    <t>alle Umzüge aus Umlandregionen MV in ABL</t>
+  </si>
+  <si>
+    <t>alle Umzüge aus Umlandregionen von Rostock nach Rostock</t>
+  </si>
+  <si>
+    <t>alle Fortzüge Kreis Potsdam-Mittelmark in Kreise ABL 2004</t>
+  </si>
+  <si>
+    <t>alle Zuzüge Kreis Potsdam-Mittelmark aus Kreisen ABL 2004</t>
+  </si>
+  <si>
+    <t>alle Zuzüge auf Kreisebene von ABL zu NBL 2006</t>
+  </si>
+  <si>
+    <t>alle Zuzüge Kreis Potsdam-Mittelmark aus Kreisen ABL 2004 G:w, FS:1</t>
+  </si>
+  <si>
+    <t>Bevölkerungssaldo Sachsen-Anhalt auf Kreisebene 2000 bis 2006</t>
+  </si>
+  <si>
+    <t>Wanderungsssaldo Sachsen-Anhalt auf Kreisebene 2000 bis 2006</t>
+  </si>
+  <si>
+    <t>Wanderungsssaldo Sachsen-Anhalt auf Kreisebene 2000 bis 2006/EW</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>Definition der Umlandregionen aus Pendlerrate zu Oberzentren(Zone1&gt;= 40%; zone2&gt;=20%) - Pendlerdaten 2006 benötigt</t>
+  </si>
+  <si>
+    <t>?Definition Umlandkreise?</t>
+  </si>
+  <si>
+    <t>alle Kreise BB mit Wanderungssaldo/EW von &gt;2%</t>
+  </si>
+  <si>
+    <t>alle Fortzüge Thüringen in ABL 2003</t>
+  </si>
+  <si>
+    <t>alle Zuzüge Thüringen aus ABL 2003</t>
+  </si>
+  <si>
+    <t>alle Fortzüge Thüringen in ABL 2003 G:w, FS:1</t>
+  </si>
+  <si>
+    <t>Bevölkerungssaldos BL</t>
+  </si>
+  <si>
+    <t>Wanderungssaldos NBL</t>
+  </si>
+  <si>
+    <t>Wanderungssaldos NBL/EW</t>
+  </si>
+  <si>
+    <t>allgemeine, einfache  Abfragen</t>
+  </si>
+  <si>
+    <t>Bevölkerungsstand 2000 bis 2009 Deutschland</t>
+  </si>
+  <si>
+    <t>Bevölkerungsstand 2000 bis 2009 Sachsen</t>
+  </si>
+  <si>
+    <t>Bevölkerungsstand 2000 bis 2009 Gemeinde (14729)</t>
+  </si>
+  <si>
+    <t>Bevölkerungsstand 2000 bis 2009 Gemeinde Wurzen, Stadt (14729410)</t>
+  </si>
+  <si>
+    <t>Bevölkerungsstand D 2000 nach BL</t>
+  </si>
+  <si>
+    <t>Bevölkerungsstand D 2000 nach Kreisen</t>
+  </si>
+  <si>
+    <t>Bevölkerungsstand D 2000 nach Gemeinden</t>
+  </si>
+  <si>
+    <t>Umzüge D 2000 nach NBL</t>
   </si>
 </sst>
 </file>
@@ -568,15 +655,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F39"/>
+  <dimension ref="A1:F48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="D49" sqref="D49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25" customWidth="1"/>
+    <col min="1" max="1" width="28" customWidth="1"/>
     <col min="2" max="2" width="66.140625" style="4" customWidth="1"/>
     <col min="3" max="3" width="15.85546875" customWidth="1"/>
     <col min="4" max="4" width="74.42578125" customWidth="1"/>
@@ -727,118 +814,224 @@
         <v>58</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>32</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D17" s="4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B18" s="4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D18" s="4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B19" s="4" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="D19" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B20" s="4" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D20" s="4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B21" s="4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D21" s="4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>31</v>
       </c>
       <c r="B23" s="4" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D23" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B24" s="5" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D24" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B25" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D25" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B26" s="4" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D26" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B27" s="5" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D27" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B28" s="5" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="D28" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B29" s="4" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="D29" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B30" s="4" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D30" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B31" s="4" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D31" s="4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B32" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D32" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>33</v>
       </c>
       <c r="B34" s="4" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D34" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B35" s="5" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D35" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B36" s="4" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D36" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B37" s="4" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D37" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B38" s="5" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D38" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B39" s="5" t="s">
         <v>30</v>
+      </c>
+      <c r="D39" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>79</v>
+      </c>
+      <c r="D41" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D42" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D43" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D44" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D45" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D46" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D47" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D48" t="s">
+        <v>87</v>
       </c>
     </row>
   </sheetData>

</xml_diff>